<commit_message>
Update to cbs race extension and patient example.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cbs-race.xlsx
+++ b/output/StructureDefinition-cbs-race.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$30</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="97">
   <si>
     <t>Path</t>
   </si>
@@ -137,7 +137,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>US Core Race Extension</t>
+    <t>CBS Race Extension</t>
   </si>
   <si>
     <t>Concepts classifying the person into a named category of humans sharing common history, traits, geographical origin or nationality.  The race codes used to represent these concepts are based upon the [CDC Race and Ethnicity Code Set Version 1.0](http://www.cdc.gov/phin/resources/vocabulary/index.html) which includes over 900 concepts for representing race and ethnicity of which 921 reference race.  The race concepts are grouped by and pre-mapped to the 5 OMB race categories:
@@ -210,7 +210,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t>American Indian or Alaska Native|Asian|Black or African American|Native Hawaiian or Other Pacific Islander|White</t>
+    <t>American Indian or Alaska Native|Asian|Black or African American|Native Hawaiian or Other Pacific Islander|White as well as null flavors</t>
   </si>
   <si>
     <t>The 5 race category codes according to the [OMB Standards for Maintaining, Collecting, and Presenting Federal Data on Race and Ethnicity, Statistical Policy Directive No. 15, as revised, October 30, 1997](https://www.govinfo.gov/content/pkg/FR-1997-10-30/pdf/97-28653.pdf).</t>
@@ -277,7 +277,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/ValueSet/omb-race-category</t>
+    <t>http://phinvads.cdc.gov/fhir/ValueSet/2.16.840.1.114222.4.11.7205</t>
   </si>
   <si>
     <t>detailed</t>
@@ -295,6 +295,18 @@
     <t>http://hl7.org/fhir/us/core/ValueSet/detailed-race</t>
   </si>
   <si>
+    <t>otherRace</t>
+  </si>
+  <si>
+    <t>Other Race</t>
+  </si>
+  <si>
+    <t>Other race text provided for continuity with Generic v2.0 Message Mapping Guides.</t>
+  </si>
+  <si>
+    <t>valueString</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
@@ -302,9 +314,6 @@
   </si>
   <si>
     <t>Plain text representation of the race concept(s).</t>
-  </si>
-  <si>
-    <t>valueString</t>
   </si>
   <si>
     <t>http://cbsig.chai.gatech.edu/output/StructureDefinition/cbs-race</t>
@@ -460,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ24"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -479,7 +488,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="101.99609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="121.59765625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -493,7 +502,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="251.41015625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="52.5078125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="63.4453125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
@@ -2125,7 +2134,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
         <v>51</v>
       </c>
@@ -2137,13 +2146,13 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>37</v>
@@ -2729,11 +2738,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>92</v>
+      </c>
       <c r="C23" t="s" s="2">
         <v>37</v>
       </c>
@@ -2745,7 +2756,7 @@
         <v>39</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>37</v>
@@ -2754,24 +2765,22 @@
         <v>37</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>69</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>37</v>
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" t="s" s="2">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="R23" t="s" s="2">
         <v>37</v>
@@ -2813,27 +2822,27 @@
         <v>37</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -2844,7 +2853,7 @@
         <v>38</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>37</v>
@@ -2856,13 +2865,13 @@
         <v>37</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -2913,26 +2922,630 @@
         <v>37</v>
       </c>
       <c r="AE24" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AF24" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG24" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ24" t="s" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" hidden="true">
+      <c r="A25" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F25" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J25" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K25" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="L25" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA25" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AB25" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AC25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD25" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AE25" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AF25" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG25" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI25" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ25" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" hidden="true">
+      <c r="A26" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F26" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="G26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J26" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="N26" s="2"/>
+      <c r="O26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P26" s="2"/>
+      <c r="Q26" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="R26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE26" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AF26" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG26" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ26" t="s" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" hidden="true">
+      <c r="A27" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F27" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="G27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="K27" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="L27" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB27" s="2"/>
+      <c r="AC27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE27" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="AF24" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG24" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AH24" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI24" t="s" s="2">
+      <c r="AF27" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG27" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI27" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="AJ24" t="s" s="2">
+      <c r="AJ27" t="s" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" hidden="true">
+      <c r="A28" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F28" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="G28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J28" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="K28" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P28" s="2"/>
+      <c r="Q28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE28" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AF28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG28" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI28" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" hidden="true">
+      <c r="A29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="G29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J29" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="N29" s="2"/>
+      <c r="O29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="R29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" hidden="true">
+      <c r="A30" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F30" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J30" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="K30" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE30" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AF30" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI30" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ24">
+  <autoFilter ref="A1:AJ30">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -2942,7 +3555,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI23">
+  <conditionalFormatting sqref="A2:AI29">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Validation workaround for race extension.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cbs-race.xlsx
+++ b/output/StructureDefinition-cbs-race.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="102">
   <si>
     <t>Path</t>
   </si>
@@ -181,11 +181,21 @@
     <t>Extension.extension</t>
   </si>
   <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>An Extension</t>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
     <t xml:space="preserve">value:url}
@@ -222,6 +232,9 @@
     <t>Extension.extension.extension</t>
   </si>
   <si>
+    <t>An Extension</t>
+  </si>
+  <si>
     <t>Extension.extension.url</t>
   </si>
   <si>
@@ -274,19 +287,22 @@
     <t>valueCoding</t>
   </si>
   <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>http://phinvads.cdc.gov/fhir/ValueSet/2.16.840.1.114222.4.11.7205</t>
+  </si>
+  <si>
+    <t>detailed</t>
+  </si>
+  <si>
+    <t>Extended race codes</t>
+  </si>
+  <si>
+    <t>The 900+ CDC race codes that are grouped under one of the 5 OMB race category codes:.</t>
+  </si>
+  <si>
     <t>required</t>
-  </si>
-  <si>
-    <t>http://phinvads.cdc.gov/fhir/ValueSet/2.16.840.1.114222.4.11.7205</t>
-  </si>
-  <si>
-    <t>detailed</t>
-  </si>
-  <si>
-    <t>Extended race codes</t>
-  </si>
-  <si>
-    <t>The 900+ CDC race codes that are grouped under one of the 5 OMB race category codes:.</t>
   </si>
   <si>
     <t>The [900+ CDC Race codes](http://www.cdc.gov/phin/resources/vocabulary/index.html) that are grouped under one of the 5 OMB race category codes.</t>
@@ -480,7 +496,7 @@
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="13.0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.16796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="12.19921875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
@@ -832,11 +848,11 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s" s="2">
         <v>42</v>
@@ -851,15 +867,17 @@
         <v>37</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="M4" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="M4" t="s" s="2">
+        <v>56</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>37</v>
@@ -896,19 +914,19 @@
         <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>38</v>
@@ -923,7 +941,7 @@
         <v>44</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -931,7 +949,7 @@
         <v>51</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>37</v>
@@ -941,10 +959,10 @@
         <v>38</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>37</v>
@@ -953,13 +971,13 @@
         <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1010,7 +1028,7 @@
         <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>38</v>
@@ -1030,7 +1048,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1130,7 +1148,7 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -1153,13 +1171,13 @@
         <v>37</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1198,19 +1216,19 @@
         <v>37</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AC7" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD7" t="s" s="2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>38</v>
@@ -1230,7 +1248,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -1253,16 +1271,16 @@
         <v>37</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -1270,7 +1288,7 @@
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" t="s" s="2">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="R8" t="s" s="2">
         <v>37</v>
@@ -1312,7 +1330,7 @@
         <v>37</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>39</v>
@@ -1327,12 +1345,12 @@
         <v>37</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -1355,13 +1373,13 @@
         <v>37</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1400,17 +1418,17 @@
         <v>37</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>38</v>
@@ -1422,18 +1440,18 @@
         <v>37</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>37</v>
@@ -1455,13 +1473,13 @@
         <v>37</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1488,32 +1506,32 @@
         <v>37</v>
       </c>
       <c r="W10" t="s" s="2">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="X10" t="s" s="2">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="Y10" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="Z10" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA10" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB10" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC10" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD10" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE10" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="Z10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE10" t="s" s="2">
-        <v>78</v>
-      </c>
       <c r="AF10" t="s" s="2">
         <v>38</v>
       </c>
@@ -1524,10 +1542,10 @@
         <v>37</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" hidden="true">
@@ -1535,7 +1553,7 @@
         <v>51</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s" s="2">
         <v>37</v>
@@ -1557,13 +1575,13 @@
         <v>37</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1614,7 +1632,7 @@
         <v>37</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>38</v>
@@ -1634,7 +1652,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1734,7 +1752,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -1757,13 +1775,13 @@
         <v>37</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K13" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1802,19 +1820,19 @@
         <v>37</v>
       </c>
       <c r="AA13" t="s" s="2">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AC13" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD13" t="s" s="2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>38</v>
@@ -1834,7 +1852,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -1857,16 +1875,16 @@
         <v>37</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -1874,7 +1892,7 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" t="s" s="2">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="R14" t="s" s="2">
         <v>37</v>
@@ -1916,7 +1934,7 @@
         <v>37</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>39</v>
@@ -1931,12 +1949,12 @@
         <v>37</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -1959,13 +1977,13 @@
         <v>37</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2004,17 +2022,17 @@
         <v>37</v>
       </c>
       <c r="AA15" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AB15" s="2"/>
       <c r="AC15" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>38</v>
@@ -2026,18 +2044,18 @@
         <v>37</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>37</v>
@@ -2059,13 +2077,13 @@
         <v>37</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2092,13 +2110,13 @@
         <v>37</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>37</v>
@@ -2116,7 +2134,7 @@
         <v>37</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>38</v>
@@ -2128,10 +2146,10 @@
         <v>37</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" hidden="true">
@@ -2139,7 +2157,7 @@
         <v>51</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>37</v>
@@ -2161,13 +2179,13 @@
         <v>37</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2218,7 +2236,7 @@
         <v>37</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>38</v>
@@ -2238,7 +2256,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2338,7 +2356,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2361,13 +2379,13 @@
         <v>37</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K19" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2406,19 +2424,19 @@
         <v>37</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AB19" t="s" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AC19" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD19" t="s" s="2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>38</v>
@@ -2438,7 +2456,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2461,16 +2479,16 @@
         <v>37</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -2478,7 +2496,7 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" t="s" s="2">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="R20" t="s" s="2">
         <v>37</v>
@@ -2520,7 +2538,7 @@
         <v>37</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
@@ -2535,12 +2553,12 @@
         <v>37</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -2566,10 +2584,10 @@
         <v>46</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2608,17 +2626,17 @@
         <v>37</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AB21" s="2"/>
       <c r="AC21" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>38</v>
@@ -2630,18 +2648,18 @@
         <v>37</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>37</v>
@@ -2666,10 +2684,10 @@
         <v>46</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -2720,7 +2738,7 @@
         <v>37</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>38</v>
@@ -2732,10 +2750,10 @@
         <v>37</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23">
@@ -2743,20 +2761,20 @@
         <v>51</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>37</v>
@@ -2765,13 +2783,13 @@
         <v>37</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2822,7 +2840,7 @@
         <v>37</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>38</v>
@@ -2842,7 +2860,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -2942,7 +2960,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -2965,13 +2983,13 @@
         <v>37</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K25" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -3010,19 +3028,19 @@
         <v>37</v>
       </c>
       <c r="AA25" t="s" s="2">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AB25" t="s" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AC25" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD25" t="s" s="2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>38</v>
@@ -3042,7 +3060,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3065,16 +3083,16 @@
         <v>37</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
@@ -3082,7 +3100,7 @@
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" t="s" s="2">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="R26" t="s" s="2">
         <v>37</v>
@@ -3124,7 +3142,7 @@
         <v>37</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>39</v>
@@ -3139,12 +3157,12 @@
         <v>37</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3170,10 +3188,10 @@
         <v>46</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -3212,17 +3230,17 @@
         <v>37</v>
       </c>
       <c r="AA27" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AB27" s="2"/>
       <c r="AC27" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD27" t="s" s="2">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>38</v>
@@ -3234,18 +3252,18 @@
         <v>37</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s" s="2">
         <v>37</v>
@@ -3270,10 +3288,10 @@
         <v>46</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -3324,7 +3342,7 @@
         <v>37</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>38</v>
@@ -3336,15 +3354,15 @@
         <v>37</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -3367,16 +3385,16 @@
         <v>37</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -3384,7 +3402,7 @@
       </c>
       <c r="P29" s="2"/>
       <c r="Q29" t="s" s="2">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="R29" t="s" s="2">
         <v>37</v>
@@ -3426,7 +3444,7 @@
         <v>37</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>39</v>
@@ -3441,12 +3459,12 @@
         <v>37</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -3469,13 +3487,13 @@
         <v>37</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -3526,7 +3544,7 @@
         <v>37</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>38</v>
@@ -3538,10 +3556,10 @@
         <v>37</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>